<commit_message>
Atualização da cor do texto
</commit_message>
<xml_diff>
--- a/controle de trafego(frota terceirizada) planilha 1.xlsx
+++ b/controle de trafego(frota terceirizada) planilha 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno.vargas\Desktop\PROJETOS\dashboard-dtran-nov25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F4F5C3-61E9-47EC-9F57-ED5C666B62E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3C7644-A22F-4D5C-B882-558EF4C0B121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="2535" windowWidth="20730" windowHeight="11160" tabRatio="808" xr2:uid="{A8503064-5735-4A81-AD91-8CF0BC577997}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="808" activeTab="1" xr2:uid="{A8503064-5735-4A81-AD91-8CF0BC577997}"/>
   </bookViews>
   <sheets>
     <sheet name="PEDIDOS ATENDIDOS" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PEDIDOS ATENDIDOS'!$A$1:$B$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'TEMPO EM PERNOITE'!$A$1:$B$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'TEMPO EM PERNOITE'!$A$1:$B$8</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>SUPED</t>
   </si>
@@ -950,9 +950,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'TEMPO EM PERNOITE'!$A$2:$A$9</c:f>
+              <c:f>'TEMPO EM PERNOITE'!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>SUPED</c:v>
                 </c:pt>
@@ -963,18 +963,15 @@
                   <c:v>GABINETE</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>SUART</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>COGESPA</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>SUART</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>SUART</c:v>
+                  <c:v>DIISE</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>DIISE</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>DIPLIC</c:v>
                 </c:pt>
               </c:strCache>
@@ -982,10 +979,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'TEMPO EM PERNOITE'!$B$2:$B$9</c:f>
+              <c:f>'TEMPO EM PERNOITE'!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -996,7 +993,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2</c:v>
@@ -1005,9 +1002,6 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -2369,7 +2363,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2719,7 +2713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23140D4E-4344-4026-B946-26330EA60A39}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -2876,10 +2870,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00BEEE4-0E55-463E-BE77-9C71403AEE3B}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2926,15 +2920,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" s="5">
         <v>2</v>
@@ -2942,7 +2936,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="5">
         <v>1</v>
@@ -2950,37 +2944,29 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5">
-        <v>1</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3">
-        <f>SUM(B2:B9)</f>
+      <c r="B10" s="3">
+        <f>SUM(B2:B8)</f>
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B9" xr:uid="{23140D4E-4344-4026-B946-26330EA60A39}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B9">
-      <sortCondition descending="1" ref="B1:B9"/>
+  <autoFilter ref="A1:B8" xr:uid="{23140D4E-4344-4026-B946-26330EA60A39}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B8">
+      <sortCondition descending="1" ref="B1:B8"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>